<commit_message>
added benchmarking to code and doc
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaackim/Desktop/Projects/SIP_SoftwarePipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47385923-0385-AF48-8087-B75696E53435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEC7901-D81E-1C4B-A0F5-496EB7035C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17440" xr2:uid="{398766A5-0F43-C549-9981-7256F5067925}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Functional Kalman C++</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Trial (μs)</t>
+  </si>
+  <si>
+    <t>Kalman with Eigen C++ (AvgTime for 1000 Runs)</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF7E80B-9E4B-0A46-AB12-1250715D2C61}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -436,10 +439,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="3" max="4" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -449,8 +452,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -460,8 +466,11 @@
       <c r="C2">
         <v>26.709</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>48.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -471,8 +480,11 @@
       <c r="C3">
         <v>67.209000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>57.07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -482,8 +494,11 @@
       <c r="C4">
         <v>72.209000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>61.999000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -493,8 +508,11 @@
       <c r="C5">
         <v>89.415999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>59.22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -504,8 +522,11 @@
       <c r="C6">
         <v>79.332999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>62.826999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -515,8 +536,11 @@
       <c r="C7">
         <v>48.834000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>56.926000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -526,8 +550,11 @@
       <c r="C8">
         <v>65.082999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>58.396999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -537,8 +564,11 @@
       <c r="C9">
         <v>83.165999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>55.204000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -548,8 +578,11 @@
       <c r="C10">
         <v>75.292000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>56.713999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -559,8 +592,11 @@
       <c r="C11">
         <v>73.792000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>56.73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -571,6 +607,10 @@
       <c r="C12">
         <f>AVERAGE(C2:C11)</f>
         <v>68.104300000000009</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(D2:D11)</f>
+        <v>57.393700000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
benchmarked functional kalman with python
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaackim/Desktop/Projects/SIP_SoftwarePipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEC7901-D81E-1C4B-A0F5-496EB7035C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393AD067-2B01-4F44-B125-6387768C16C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17440" xr2:uid="{398766A5-0F43-C549-9981-7256F5067925}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Functional Kalman C++</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Kalman with Eigen C++ (AvgTime for 1000 Runs)</t>
+  </si>
+  <si>
+    <t>Functional Kalman Python</t>
   </si>
 </sst>
 </file>
@@ -430,19 +433,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF7E80B-9E4B-0A46-AB12-1250715D2C61}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -455,8 +459,11 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -469,8 +476,11 @@
       <c r="D2">
         <v>48.85</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>355.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -483,8 +493,11 @@
       <c r="D3">
         <v>57.07</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>77.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -497,8 +510,11 @@
       <c r="D4">
         <v>61.999000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>91.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -511,8 +527,11 @@
       <c r="D5">
         <v>59.22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>60.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -525,8 +544,11 @@
       <c r="D6">
         <v>62.826999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>60.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -539,8 +561,11 @@
       <c r="D7">
         <v>56.926000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>66.040000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -553,8 +578,11 @@
       <c r="D8">
         <v>58.396999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>82.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -567,8 +595,11 @@
       <c r="D9">
         <v>55.204000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>83.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -581,8 +612,11 @@
       <c r="D10">
         <v>56.713999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>94.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -595,8 +629,11 @@
       <c r="D11">
         <v>56.73</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>56.74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -611,6 +648,10 @@
       <c r="D12">
         <f>AVERAGE(D2:D11)</f>
         <v>57.393700000000003</v>
+      </c>
+      <c r="E12">
+        <f>AVERAGE(E2:E11)</f>
+        <v>102.73500000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
got kalman object oriented version working in python
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaackim/Desktop/Projects/SIP_SoftwarePipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393AD067-2B01-4F44-B125-6387768C16C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25C80AE-B052-CA43-BFDA-7D3A72136993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17440" xr2:uid="{398766A5-0F43-C549-9981-7256F5067925}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Functional Kalman C++</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Functional Kalman Python</t>
+  </si>
+  <si>
+    <t>Object-Oriented Kalman Python</t>
+  </si>
+  <si>
+    <t>Kalman with Eigen Python (AvgTime for 1000 Runs)</t>
   </si>
 </sst>
 </file>
@@ -433,20 +439,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF7E80B-9E4B-0A46-AB12-1250715D2C61}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="5" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -462,8 +469,14 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -479,8 +492,11 @@
       <c r="E2">
         <v>355.01</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>158.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -496,8 +512,11 @@
       <c r="E3">
         <v>77.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>74.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -513,8 +532,11 @@
       <c r="E4">
         <v>91.08</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>59.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -530,8 +552,11 @@
       <c r="E5">
         <v>60.08</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>52.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -547,8 +572,11 @@
       <c r="E6">
         <v>60.08</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>59.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -564,8 +592,11 @@
       <c r="E7">
         <v>66.040000000000006</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>49.11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -581,8 +612,11 @@
       <c r="E8">
         <v>82.97</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>49.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -598,8 +632,11 @@
       <c r="E9">
         <v>83.21</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>52.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -615,8 +652,11 @@
       <c r="E10">
         <v>94.89</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>55.79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -632,8 +672,11 @@
       <c r="E11">
         <v>56.74</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>54.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -652,6 +695,14 @@
       <c r="E12">
         <f>AVERAGE(E2:E11)</f>
         <v>102.73500000000001</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:G12" si="0">AVERAGE(F2:F11)</f>
+        <v>66.518000000000001</v>
+      </c>
+      <c r="G12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>